<commit_message>
Initial commit of momentum project
</commit_message>
<xml_diff>
--- a/23:24/PLteamsData23:24_updated.xlsx
+++ b/23:24/PLteamsData23:24_updated.xlsx
@@ -18,14 +18,14 @@
     <sheet name="Everton" sheetId="9" r:id="rId9"/>
     <sheet name="Fulham" sheetId="10" r:id="rId10"/>
     <sheet name="Liverpool" sheetId="11" r:id="rId11"/>
-    <sheet name="Luton Town" sheetId="12" r:id="rId12"/>
-    <sheet name="Manchester City" sheetId="13" r:id="rId13"/>
-    <sheet name="Manchester United" sheetId="14" r:id="rId14"/>
-    <sheet name="Newcastle United" sheetId="15" r:id="rId15"/>
-    <sheet name="Nottingham Forest" sheetId="16" r:id="rId16"/>
-    <sheet name="Sheffield United" sheetId="17" r:id="rId17"/>
-    <sheet name="Tottenham Hotspur" sheetId="18" r:id="rId18"/>
-    <sheet name="West Ham United" sheetId="19" r:id="rId19"/>
+    <sheet name="Luton" sheetId="12" r:id="rId12"/>
+    <sheet name="Man City" sheetId="13" r:id="rId13"/>
+    <sheet name="Man Utd" sheetId="14" r:id="rId14"/>
+    <sheet name="Newcastle" sheetId="15" r:id="rId15"/>
+    <sheet name="Nott'm Forest" sheetId="16" r:id="rId16"/>
+    <sheet name="Sheffield Utd" sheetId="17" r:id="rId17"/>
+    <sheet name="Spurs" sheetId="18" r:id="rId18"/>
+    <sheet name="West Ham" sheetId="19" r:id="rId19"/>
     <sheet name="Wolves" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3260" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3278" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>Corrected Win Rate After 2 Wins</t>
   </si>
   <si>
     <t>Total Wins in Momentum</t>
@@ -609,7 +612,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1517,7 +1520,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1525,15 +1531,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>0</v>
+      <c r="F42">
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1541,6 +1547,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>1</v>
       </c>
     </row>
@@ -1551,7 +1565,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1614,7 +1628,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -1631,7 +1645,7 @@
         <v>26.8</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -1660,7 +1674,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
@@ -1844,7 +1858,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
@@ -1890,7 +1904,7 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
@@ -1959,7 +1973,7 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
         <v>47</v>
@@ -2005,7 +2019,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -2022,7 +2036,7 @@
         <v>31.12</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
@@ -2258,7 +2272,7 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E31" t="s">
         <v>46</v>
@@ -2281,7 +2295,7 @@
         <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E32" t="s">
         <v>47</v>
@@ -2350,7 +2364,7 @@
         <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E35" t="s">
         <v>47</v>
@@ -2419,7 +2433,7 @@
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E38" t="s">
         <v>47</v>
@@ -2442,7 +2456,7 @@
         <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E39" t="s">
         <v>45</v>
@@ -2461,21 +2475,24 @@
       <c r="F40">
         <v>0</v>
       </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="E41" t="s">
         <v>49</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>1</v>
+      <c r="F42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2483,6 +2500,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>3</v>
       </c>
     </row>
@@ -2493,7 +2518,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2918,7 +2943,7 @@
         <v>23.12</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -2970,7 +2995,7 @@
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
         <v>45</v>
@@ -3033,13 +3058,13 @@
         <v>4.2</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
@@ -3338,7 +3363,7 @@
         <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E37" t="s">
         <v>45</v>
@@ -3361,7 +3386,7 @@
         <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
         <v>46</v>
@@ -3401,7 +3426,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -3409,15 +3437,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>0</v>
+      <c r="F42">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3425,6 +3453,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>0</v>
       </c>
     </row>
@@ -3435,7 +3471,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3475,7 +3511,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>
@@ -3498,7 +3534,7 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -3682,7 +3718,7 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
@@ -3774,7 +3810,7 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
@@ -3791,13 +3827,13 @@
         <v>5.12</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
@@ -3889,7 +3925,7 @@
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -3958,7 +3994,7 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
         <v>46</v>
@@ -3981,7 +4017,7 @@
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
@@ -4027,7 +4063,7 @@
         <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
         <v>47</v>
@@ -4050,7 +4086,7 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
         <v>47</v>
@@ -4096,7 +4132,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E29" t="s">
         <v>47</v>
@@ -4159,7 +4195,7 @@
         <v>3.4</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
         <v>27</v>
@@ -4211,7 +4247,7 @@
         <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
         <v>47</v>
@@ -4234,7 +4270,7 @@
         <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E35" t="s">
         <v>47</v>
@@ -4303,7 +4339,7 @@
         <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E38" t="s">
         <v>47</v>
@@ -4326,7 +4362,7 @@
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
         <v>47</v>
@@ -4345,21 +4381,24 @@
       <c r="F40">
         <v>0</v>
       </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="E41" t="s">
         <v>49</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>6</v>
+      <c r="F42">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -4368,6 +4407,14 @@
       </c>
       <c r="G43">
         <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -4377,7 +4424,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4486,7 +4533,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
@@ -4572,7 +4619,7 @@
         <v>8.1</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -4647,7 +4694,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
         <v>45</v>
@@ -4670,7 +4717,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
         <v>46</v>
@@ -4716,7 +4763,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>46</v>
@@ -5055,7 +5102,7 @@
         <v>31.3</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
         <v>26</v>
@@ -5107,7 +5154,7 @@
         <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E32" t="s">
         <v>45</v>
@@ -5130,7 +5177,7 @@
         <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E33" t="s">
         <v>45</v>
@@ -5199,7 +5246,7 @@
         <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E36" t="s">
         <v>45</v>
@@ -5285,7 +5332,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>17</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -5293,15 +5343,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>0</v>
+      <c r="F42">
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -5309,6 +5359,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>1</v>
       </c>
     </row>
@@ -5319,7 +5377,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5422,13 +5480,13 @@
         <v>3.9</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
@@ -5451,7 +5509,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -5566,7 +5624,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
@@ -5704,7 +5762,7 @@
         <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
@@ -5957,7 +6015,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
@@ -6026,7 +6084,7 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
         <v>47</v>
@@ -6095,7 +6153,7 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E34" t="s">
         <v>45</v>
@@ -6141,7 +6199,7 @@
         <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E36" t="s">
         <v>47</v>
@@ -6158,7 +6216,7 @@
         <v>12.5</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
         <v>26</v>
@@ -6227,7 +6285,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -6242,8 +6303,8 @@
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>0</v>
+      <c r="F42">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -6251,6 +6312,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>3</v>
       </c>
     </row>
@@ -6261,7 +6330,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6301,7 +6370,7 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
@@ -6370,7 +6439,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
@@ -6416,7 +6485,7 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
@@ -6525,7 +6594,7 @@
         <v>4.11</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -6623,7 +6692,7 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
@@ -6646,7 +6715,7 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
@@ -6715,7 +6784,7 @@
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -6738,7 +6807,7 @@
         <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
@@ -6761,7 +6830,7 @@
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
@@ -6807,7 +6876,7 @@
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
         <v>46</v>
@@ -6870,13 +6939,13 @@
         <v>24.2</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
         <v>47</v>
@@ -6922,7 +6991,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
         <v>47</v>
@@ -7060,7 +7129,7 @@
         <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E35" t="s">
         <v>45</v>
@@ -7129,7 +7198,7 @@
         <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
         <v>47</v>
@@ -7152,7 +7221,7 @@
         <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E39" t="s">
         <v>45</v>
@@ -7169,7 +7238,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -7177,15 +7249,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>3</v>
+      <c r="F42">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -7193,6 +7265,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>3</v>
       </c>
     </row>
@@ -7203,7 +7283,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7237,7 +7317,7 @@
         <v>12.8</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -7289,7 +7369,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
@@ -7450,7 +7530,7 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
@@ -7496,7 +7576,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
@@ -7519,7 +7599,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
@@ -7565,7 +7645,7 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
@@ -7634,7 +7714,7 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
@@ -7703,7 +7783,7 @@
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
@@ -7720,7 +7800,7 @@
         <v>30.1</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
         <v>26</v>
@@ -7772,7 +7852,7 @@
         <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
         <v>47</v>
@@ -7818,7 +7898,7 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
         <v>47</v>
@@ -7956,7 +8036,7 @@
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
         <v>47</v>
@@ -8071,7 +8151,7 @@
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
         <v>47</v>
@@ -8113,21 +8193,24 @@
       <c r="F40">
         <v>0</v>
       </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="E41" t="s">
         <v>49</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>3</v>
+      <c r="F42">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -8135,6 +8218,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>5</v>
       </c>
     </row>
@@ -8300,7 +8391,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
@@ -8346,7 +8437,7 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
@@ -8386,13 +8477,13 @@
         <v>28.1</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
@@ -8461,7 +8552,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
@@ -8484,7 +8575,7 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
@@ -8599,7 +8690,7 @@
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -8668,7 +8759,7 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
@@ -8691,7 +8782,7 @@
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
@@ -8737,7 +8828,7 @@
         <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
         <v>47</v>
@@ -8777,13 +8868,13 @@
         <v>4.3</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
@@ -8829,7 +8920,7 @@
         <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
         <v>46</v>
@@ -8852,7 +8943,7 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E31" t="s">
         <v>47</v>
@@ -8921,7 +9012,7 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
         <v>47</v>
@@ -8944,7 +9035,7 @@
         <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E35" t="s">
         <v>47</v>
@@ -8967,7 +9058,7 @@
         <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E36" t="s">
         <v>47</v>
@@ -8990,7 +9081,7 @@
         <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E37" t="s">
         <v>47</v>
@@ -9036,7 +9127,7 @@
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
         <v>47</v>
@@ -9050,7 +9141,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="E40" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -9058,7 +9149,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="E41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -9066,7 +9157,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G42">
         <v>12</v>
@@ -9074,7 +9165,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="E43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G43">
         <v>6</v>
@@ -9087,7 +9178,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9196,7 +9287,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
@@ -9236,7 +9327,7 @@
         <v>24.9</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
@@ -9357,7 +9448,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
@@ -9426,7 +9517,7 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>46</v>
@@ -9541,7 +9632,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -9748,7 +9839,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
         <v>47</v>
@@ -9840,7 +9931,7 @@
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
         <v>47</v>
@@ -9857,13 +9948,13 @@
         <v>28.4</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
         <v>47</v>
@@ -9909,7 +10000,7 @@
         <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s">
         <v>47</v>
@@ -9995,7 +10086,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -10003,15 +10097,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>3</v>
+      <c r="F42">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -10019,6 +10113,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>2</v>
       </c>
     </row>
@@ -10029,7 +10131,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10161,7 +10263,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -10184,7 +10286,7 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
@@ -10253,7 +10355,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
         <v>47</v>
@@ -10299,7 +10401,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
@@ -10414,7 +10516,7 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
@@ -10477,7 +10579,7 @@
         <v>28.12</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
@@ -10575,7 +10677,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
@@ -10592,13 +10694,13 @@
         <v>11.2</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E25" t="s">
         <v>47</v>
@@ -10644,7 +10746,7 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
         <v>45</v>
@@ -10736,7 +10838,7 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
         <v>47</v>
@@ -10828,7 +10930,7 @@
         <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E35" t="s">
         <v>47</v>
@@ -10874,7 +10976,7 @@
         <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E37" t="s">
         <v>47</v>
@@ -10920,7 +11022,7 @@
         <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E39" t="s">
         <v>47</v>
@@ -10937,7 +11039,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -10945,15 +11050,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>2</v>
+      <c r="F42">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -10961,6 +11066,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>4</v>
       </c>
     </row>
@@ -10971,7 +11084,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11011,7 +11124,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>
@@ -11080,7 +11193,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
@@ -11149,7 +11262,7 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
         <v>45</v>
@@ -11350,7 +11463,7 @@
         <v>9.119999999999999</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -11425,7 +11538,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -11494,7 +11607,7 @@
         <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
@@ -11586,7 +11699,7 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
         <v>45</v>
@@ -11632,7 +11745,7 @@
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
         <v>47</v>
@@ -11701,7 +11814,7 @@
         <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
         <v>47</v>
@@ -11724,7 +11837,7 @@
         <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E33" t="s">
         <v>46</v>
@@ -11741,7 +11854,7 @@
         <v>14.4</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
         <v>27</v>
@@ -11839,7 +11952,7 @@
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
         <v>46</v>
@@ -11862,7 +11975,7 @@
         <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E39" t="s">
         <v>47</v>
@@ -11879,7 +11992,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -11887,15 +12003,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>0</v>
+      <c r="F42">
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -11903,6 +12019,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>0</v>
       </c>
     </row>
@@ -11913,7 +12037,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11976,7 +12100,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -12022,7 +12146,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
@@ -12045,7 +12169,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -12229,7 +12353,7 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
@@ -12246,7 +12370,7 @@
         <v>2.12</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -12321,7 +12445,7 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
         <v>47</v>
@@ -12436,7 +12560,7 @@
         <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
@@ -12459,7 +12583,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
         <v>45</v>
@@ -12551,7 +12675,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
@@ -12683,7 +12807,7 @@
         <v>20.4</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
         <v>26</v>
@@ -12758,7 +12882,7 @@
         <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E37" t="s">
         <v>47</v>
@@ -12781,7 +12905,7 @@
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E38" t="s">
         <v>47</v>
@@ -12821,7 +12945,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -12829,15 +12956,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>1</v>
+      <c r="F42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -12845,7 +12972,15 @@
         <v>51</v>
       </c>
       <c r="G43">
-        <v>4</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -12855,7 +12990,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -12918,7 +13053,7 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -13010,7 +13145,7 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
@@ -13027,13 +13162,13 @@
         <v>30.9</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
         <v>47</v>
@@ -13056,7 +13191,7 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
@@ -13125,7 +13260,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
@@ -13309,7 +13444,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -13332,7 +13467,7 @@
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
@@ -13401,7 +13536,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
@@ -13631,7 +13766,7 @@
         <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E34" t="s">
         <v>47</v>
@@ -13694,13 +13829,13 @@
         <v>4.5</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
         <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
         <v>47</v>
@@ -13763,7 +13898,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -13771,15 +13909,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>3</v>
+      <c r="F42">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -13788,6 +13926,14 @@
       </c>
       <c r="G43">
         <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -13797,7 +13943,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -13952,7 +14098,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
@@ -14090,7 +14236,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
@@ -14107,7 +14253,7 @@
         <v>25.11</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -14228,7 +14374,7 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
@@ -14251,7 +14397,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -14297,7 +14443,7 @@
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
@@ -14320,7 +14466,7 @@
         <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
@@ -14366,7 +14512,7 @@
         <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
         <v>47</v>
@@ -14412,7 +14558,7 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
         <v>47</v>
@@ -14452,7 +14598,7 @@
         <v>9.300000000000001</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
         <v>27</v>
@@ -14550,7 +14696,7 @@
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E33" t="s">
         <v>46</v>
@@ -14596,7 +14742,7 @@
         <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E35" t="s">
         <v>45</v>
@@ -14688,7 +14834,7 @@
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
         <v>47</v>
@@ -14705,7 +14851,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -14713,15 +14862,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>4</v>
+      <c r="F42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -14729,6 +14878,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>6</v>
       </c>
     </row>
@@ -14739,7 +14896,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14825,7 +14982,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
@@ -14917,7 +15074,7 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
         <v>47</v>
@@ -15078,7 +15235,7 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
@@ -15141,7 +15298,7 @@
         <v>17.12</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
         <v>27</v>
@@ -15193,7 +15350,7 @@
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
         <v>45</v>
@@ -15262,7 +15419,7 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
@@ -15377,7 +15534,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
@@ -15463,13 +15620,13 @@
         <v>6.4</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
         <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s">
         <v>47</v>
@@ -15515,7 +15672,7 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
         <v>47</v>
@@ -15538,7 +15695,7 @@
         <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
         <v>47</v>
@@ -15647,7 +15804,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -15655,15 +15815,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>0</v>
+      <c r="F42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -15671,7 +15831,15 @@
         <v>51</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -15721,7 +15889,7 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>
@@ -15744,7 +15912,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -15767,7 +15935,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
@@ -15882,7 +16050,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
@@ -15905,7 +16073,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
         <v>47</v>
@@ -15968,13 +16136,13 @@
         <v>11.11</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
@@ -16158,7 +16326,7 @@
         <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
@@ -16204,7 +16372,7 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
@@ -16250,7 +16418,7 @@
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
         <v>47</v>
@@ -16267,13 +16435,13 @@
         <v>17.2</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
         <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
         <v>47</v>
@@ -16296,7 +16464,7 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
         <v>47</v>
@@ -16526,7 +16694,7 @@
         <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
         <v>47</v>
@@ -16586,7 +16754,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="E40" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -16594,7 +16762,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="E41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -16602,7 +16770,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G42">
         <v>8</v>
@@ -16610,7 +16778,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="E43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G43">
         <v>5</v>
@@ -16623,7 +16791,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -16686,7 +16854,7 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -16841,7 +17009,7 @@
         <v>21.1</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -16916,7 +17084,7 @@
         <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
         <v>46</v>
@@ -16939,7 +17107,7 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
@@ -17146,7 +17314,7 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
@@ -17169,7 +17337,7 @@
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
@@ -17370,13 +17538,13 @@
         <v>23.4</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E33" t="s">
         <v>47</v>
@@ -17531,7 +17699,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -17539,15 +17710,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>0</v>
+      <c r="F42">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -17555,6 +17726,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>2</v>
       </c>
     </row>
@@ -17565,7 +17744,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17622,7 +17801,7 @@
         <v>21.8</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -17697,7 +17876,7 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -17789,7 +17968,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>47</v>
@@ -17858,7 +18037,7 @@
         <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
@@ -18059,13 +18238,13 @@
         <v>20.1</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
@@ -18111,7 +18290,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
@@ -18134,7 +18313,7 @@
         <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
         <v>47</v>
@@ -18203,7 +18382,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
@@ -18295,7 +18474,7 @@
         <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s">
         <v>47</v>
@@ -18341,7 +18520,7 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
         <v>45</v>
@@ -18473,7 +18652,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -18481,15 +18663,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>0</v>
+      <c r="F42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -18497,6 +18679,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>5</v>
       </c>
     </row>
@@ -18507,7 +18697,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -18570,7 +18760,7 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -18633,7 +18823,7 @@
         <v>17.9</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -18823,7 +19013,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
@@ -18961,7 +19151,7 @@
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -18984,7 +19174,7 @@
         <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
@@ -19145,7 +19335,7 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
@@ -19260,7 +19450,7 @@
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
         <v>47</v>
@@ -19392,7 +19582,7 @@
         <v>19.5</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>
@@ -19415,7 +19605,10 @@
         <v>48</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -19423,15 +19616,15 @@
         <v>49</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>3</v>
+      <c r="F42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -19439,6 +19632,14 @@
         <v>51</v>
       </c>
       <c r="G43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
         <v>3</v>
       </c>
     </row>

</xml_diff>